<commit_message>
added skill test 2 and 3
</commit_message>
<xml_diff>
--- a/Ex 30 - Excel Automation/ExcelAutomation/QueueItem_Example_Reports.xlsx
+++ b/Ex 30 - Excel Automation/ExcelAutomation/QueueItem_Example_Reports.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C0B526-289C-445E-B8B4-9B89DEF59BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4602F2-CBD8-461C-BF3D-3FA3BBF32D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5916" yWindow="3792" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3444" windowWidth="17280" windowHeight="8916" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="June Total" sheetId="3" r:id="rId1"/>
     <sheet name="June Report" sheetId="2" r:id="rId2"/>
-    <sheet name="July Report" sheetId="1" r:id="rId3"/>
+    <sheet name="July Total" sheetId="4" r:id="rId3"/>
+    <sheet name="July Report" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -537,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC63A2EB-C245-4ED6-AD1B-DD1B5CCE5B0C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1307,6 +1308,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EEDE7B-A04E-4E0F-8A05-16BDA789F1A0}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>35630</v>
+      </c>
+      <c r="B2">
+        <v>89075</v>
+      </c>
+      <c r="C2">
+        <v>19565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>

</xml_diff>